<commit_message>
Añadidas comparaciones con descripciones que originalmente eran de hasta 300 caracteres
</commit_message>
<xml_diff>
--- a/2. Finetuning/Descripciones_Gemini_Cortas.xlsx
+++ b/2. Finetuning/Descripciones_Gemini_Cortas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Hackaton_Biodiversidad_IA_2025\Hackathon-PNAV\2. Finetuning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\Hackathon\Hackathon-PNAV\2. Finetuning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293B6ABC-BC8C-4EF3-986B-2DA861A19767}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E06AC4E-7AD1-46EC-81EE-6F8D57BACE42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3481" uniqueCount="2273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3481" uniqueCount="2272">
   <si>
     <t>Nombres comunes</t>
   </si>
@@ -6836,9 +6836,6 @@
   </si>
   <si>
     <t>La culebra real de California es una serpiente de tamaño mediano. Las crías miden alrededor de 23 centímetros, mientras que las adultas alcanzan hasta 1 metro con 20 centímetros. Su cabeza tiene escamas grandes y fáciles de distinguir, y sus ojos son normales, no muy pequeños.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -7294,23 +7291,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K408"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G406" zoomScale="95" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J144" sqref="J144"/>
+    <sheetView tabSelected="1" topLeftCell="F255" zoomScale="95" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="J255" sqref="J255"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.81640625" style="2"/>
-    <col min="2" max="2" width="20.54296875" style="2" customWidth="1"/>
-    <col min="3" max="4" width="8.81640625" style="2"/>
-    <col min="5" max="5" width="45.81640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" style="2" customWidth="1"/>
-    <col min="7" max="9" width="45.81640625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="19.54296875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="16.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="20.5703125" style="2" customWidth="1"/>
+    <col min="3" max="4" width="8.85546875" style="2"/>
+    <col min="5" max="5" width="45.85546875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="2" customWidth="1"/>
+    <col min="7" max="9" width="45.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="19.5703125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="16.42578125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="75.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7345,7 +7342,7 @@
         <v>1412</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -7377,7 +7374,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -7412,7 +7409,7 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -7444,7 +7441,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>29</v>
       </c>
@@ -7476,7 +7473,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>35</v>
       </c>
@@ -7511,7 +7508,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>41</v>
       </c>
@@ -7543,7 +7540,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>47</v>
       </c>
@@ -7578,7 +7575,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>53</v>
       </c>
@@ -7610,7 +7607,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>59</v>
       </c>
@@ -7642,7 +7639,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>65</v>
       </c>
@@ -7674,7 +7671,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>71</v>
       </c>
@@ -7706,7 +7703,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>77</v>
       </c>
@@ -7738,7 +7735,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>83</v>
       </c>
@@ -7770,7 +7767,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>89</v>
       </c>
@@ -7802,7 +7799,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>95</v>
       </c>
@@ -7837,7 +7834,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>101</v>
       </c>
@@ -7869,7 +7866,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>107</v>
       </c>
@@ -7901,7 +7898,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>113</v>
       </c>
@@ -7933,7 +7930,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>119</v>
       </c>
@@ -7965,7 +7962,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>127</v>
       </c>
@@ -7997,7 +7994,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>133</v>
       </c>
@@ -8029,7 +8026,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>139</v>
       </c>
@@ -8061,7 +8058,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>145</v>
       </c>
@@ -8093,7 +8090,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>151</v>
       </c>
@@ -8128,7 +8125,7 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>157</v>
       </c>
@@ -8160,7 +8157,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>163</v>
       </c>
@@ -8192,7 +8189,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>169</v>
       </c>
@@ -8224,7 +8221,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>175</v>
       </c>
@@ -8256,7 +8253,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>181</v>
       </c>
@@ -8288,7 +8285,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>187</v>
       </c>
@@ -8320,7 +8317,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>193</v>
       </c>
@@ -8352,7 +8349,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>199</v>
       </c>
@@ -8384,7 +8381,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>205</v>
       </c>
@@ -8416,7 +8413,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>211</v>
       </c>
@@ -8448,7 +8445,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>217</v>
       </c>
@@ -8480,7 +8477,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>223</v>
       </c>
@@ -8512,7 +8509,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>229</v>
       </c>
@@ -8544,7 +8541,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>235</v>
       </c>
@@ -8576,7 +8573,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>241</v>
       </c>
@@ -8608,7 +8605,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>247</v>
       </c>
@@ -8640,7 +8637,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>253</v>
       </c>
@@ -8672,7 +8669,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>259</v>
       </c>
@@ -8704,7 +8701,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>265</v>
       </c>
@@ -8739,7 +8736,7 @@
         <v>1424</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2" t="s">
         <v>271</v>
       </c>
@@ -8768,7 +8765,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>276</v>
       </c>
@@ -8800,7 +8797,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>282</v>
       </c>
@@ -8832,7 +8829,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>288</v>
       </c>
@@ -8864,7 +8861,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>294</v>
       </c>
@@ -8896,7 +8893,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>300</v>
       </c>
@@ -8928,7 +8925,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>306</v>
       </c>
@@ -8960,7 +8957,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>312</v>
       </c>
@@ -8992,7 +8989,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>318</v>
       </c>
@@ -9024,7 +9021,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>324</v>
       </c>
@@ -9056,7 +9053,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>330</v>
       </c>
@@ -9088,7 +9085,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>336</v>
       </c>
@@ -9120,7 +9117,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>342</v>
       </c>
@@ -9152,7 +9149,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>348</v>
       </c>
@@ -9184,7 +9181,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>354</v>
       </c>
@@ -9216,7 +9213,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>360</v>
       </c>
@@ -9248,7 +9245,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>366</v>
       </c>
@@ -9280,7 +9277,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="62" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>372</v>
       </c>
@@ -9312,7 +9309,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>378</v>
       </c>
@@ -9344,7 +9341,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="64" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>384</v>
       </c>
@@ -9376,7 +9373,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>390</v>
       </c>
@@ -9408,7 +9405,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>396</v>
       </c>
@@ -9440,7 +9437,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>402</v>
       </c>
@@ -9472,7 +9469,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>408</v>
       </c>
@@ -9504,7 +9501,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>414</v>
       </c>
@@ -9536,7 +9533,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>420</v>
       </c>
@@ -9568,7 +9565,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>426</v>
       </c>
@@ -9600,7 +9597,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>432</v>
       </c>
@@ -9632,7 +9629,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>438</v>
       </c>
@@ -9664,7 +9661,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>444</v>
       </c>
@@ -9696,7 +9693,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>450</v>
       </c>
@@ -9728,7 +9725,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B76" s="2" t="s">
         <v>456</v>
       </c>
@@ -9760,7 +9757,7 @@
         <v>1423</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>461</v>
       </c>
@@ -9792,7 +9789,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>467</v>
       </c>
@@ -9824,7 +9821,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>473</v>
       </c>
@@ -9856,7 +9853,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>479</v>
       </c>
@@ -9888,7 +9885,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>485</v>
       </c>
@@ -9920,7 +9917,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>491</v>
       </c>
@@ -9952,7 +9949,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>497</v>
       </c>
@@ -9984,7 +9981,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>503</v>
       </c>
@@ -10016,7 +10013,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>509</v>
       </c>
@@ -10048,7 +10045,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>515</v>
       </c>
@@ -10080,7 +10077,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>521</v>
       </c>
@@ -10115,7 +10112,7 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>527</v>
       </c>
@@ -10147,7 +10144,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B89" s="2" t="s">
         <v>533</v>
       </c>
@@ -10176,7 +10173,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>538</v>
       </c>
@@ -10208,7 +10205,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>544</v>
       </c>
@@ -10240,7 +10237,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>550</v>
       </c>
@@ -10272,7 +10269,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>556</v>
       </c>
@@ -10304,7 +10301,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>562</v>
       </c>
@@ -10336,7 +10333,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>568</v>
       </c>
@@ -10368,7 +10365,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>574</v>
       </c>
@@ -10400,7 +10397,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>580</v>
       </c>
@@ -10432,7 +10429,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>586</v>
       </c>
@@ -10464,7 +10461,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>592</v>
       </c>
@@ -10496,7 +10493,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>598</v>
       </c>
@@ -10528,7 +10525,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>604</v>
       </c>
@@ -10560,7 +10557,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>610</v>
       </c>
@@ -10592,7 +10589,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>616</v>
       </c>
@@ -10624,7 +10621,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>622</v>
       </c>
@@ -10659,7 +10656,7 @@
         <v>1421</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>628</v>
       </c>
@@ -10694,7 +10691,7 @@
         <v>1420</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>634</v>
       </c>
@@ -10726,7 +10723,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>640</v>
       </c>
@@ -10758,7 +10755,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>646</v>
       </c>
@@ -10790,7 +10787,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>652</v>
       </c>
@@ -10822,7 +10819,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>658</v>
       </c>
@@ -10854,7 +10851,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>664</v>
       </c>
@@ -10886,7 +10883,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>670</v>
       </c>
@@ -10921,7 +10918,7 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>676</v>
       </c>
@@ -10956,7 +10953,7 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>682</v>
       </c>
@@ -10988,7 +10985,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>688</v>
       </c>
@@ -11020,7 +11017,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="116" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B116" s="2" t="s">
         <v>694</v>
       </c>
@@ -11049,7 +11046,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="117" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B117" s="2" t="s">
         <v>700</v>
       </c>
@@ -11078,7 +11075,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="118" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>705</v>
       </c>
@@ -11110,7 +11107,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="119" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B119" s="2" t="s">
         <v>712</v>
       </c>
@@ -11139,7 +11136,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="120" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B120" s="2" t="s">
         <v>717</v>
       </c>
@@ -11168,7 +11165,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="121" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B121" s="2" t="s">
         <v>722</v>
       </c>
@@ -11197,7 +11194,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="122" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B122" s="2" t="s">
         <v>727</v>
       </c>
@@ -11226,7 +11223,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="123" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B123" s="2" t="s">
         <v>732</v>
       </c>
@@ -11255,7 +11252,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="124" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B124" s="2" t="s">
         <v>737</v>
       </c>
@@ -11284,7 +11281,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="125" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B125" s="2" t="s">
         <v>742</v>
       </c>
@@ -11313,7 +11310,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="126" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B126" s="2" t="s">
         <v>747</v>
       </c>
@@ -11342,7 +11339,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="127" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B127" s="2" t="s">
         <v>752</v>
       </c>
@@ -11371,7 +11368,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="128" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B128" s="2" t="s">
         <v>757</v>
       </c>
@@ -11400,7 +11397,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="129" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="129" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B129" s="2" t="s">
         <v>762</v>
       </c>
@@ -11429,7 +11426,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="130" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="130" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B130" s="2" t="s">
         <v>767</v>
       </c>
@@ -11458,7 +11455,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="131" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B131" s="2" t="s">
         <v>772</v>
       </c>
@@ -11487,7 +11484,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="132" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B132" s="2" t="s">
         <v>777</v>
       </c>
@@ -11516,7 +11513,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="133" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B133" s="2" t="s">
         <v>782</v>
       </c>
@@ -11545,7 +11542,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="134" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="134" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B134" s="2" t="s">
         <v>787</v>
       </c>
@@ -11574,7 +11571,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="135" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="135" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B135" s="2" t="s">
         <v>792</v>
       </c>
@@ -11603,7 +11600,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="136" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="136" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B136" s="2" t="s">
         <v>797</v>
       </c>
@@ -11635,7 +11632,7 @@
         <v>1417</v>
       </c>
     </row>
-    <row r="137" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="137" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="2" t="s">
         <v>802</v>
       </c>
@@ -11664,7 +11661,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="138" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="138" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B138" s="2" t="s">
         <v>807</v>
       </c>
@@ -11693,7 +11690,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="139" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="139" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B139" s="2" t="s">
         <v>812</v>
       </c>
@@ -11722,7 +11719,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="140" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="140" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B140" s="2" t="s">
         <v>817</v>
       </c>
@@ -11751,7 +11748,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="141" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="141" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B141" s="2" t="s">
         <v>822</v>
       </c>
@@ -11780,7 +11777,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="142" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="142" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B142" s="2" t="s">
         <v>827</v>
       </c>
@@ -11809,7 +11806,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="143" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="143" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B143" s="2" t="s">
         <v>832</v>
       </c>
@@ -11838,7 +11835,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="144" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="144" spans="2:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B144" s="2" t="s">
         <v>837</v>
       </c>
@@ -11867,7 +11864,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="145" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="145" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B145" s="2" t="s">
         <v>842</v>
       </c>
@@ -11896,7 +11893,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="146" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="146" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B146" s="2" t="s">
         <v>847</v>
       </c>
@@ -11925,7 +11922,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="147" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="147" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B147" s="2" t="s">
         <v>852</v>
       </c>
@@ -11954,7 +11951,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="148" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="148" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B148" s="2" t="s">
         <v>857</v>
       </c>
@@ -11983,7 +11980,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="149" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="149" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B149" s="2" t="s">
         <v>862</v>
       </c>
@@ -12012,7 +12009,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="150" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="150" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B150" s="2" t="s">
         <v>867</v>
       </c>
@@ -12041,7 +12038,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="151" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B151" s="2" t="s">
         <v>872</v>
       </c>
@@ -12070,7 +12067,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="152" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="152" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B152" s="2" t="s">
         <v>877</v>
       </c>
@@ -12099,7 +12096,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="153" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="153" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B153" s="2" t="s">
         <v>882</v>
       </c>
@@ -12128,7 +12125,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="154" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="154" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B154" s="2" t="s">
         <v>887</v>
       </c>
@@ -12157,7 +12154,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="155" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="155" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B155" s="2" t="s">
         <v>892</v>
       </c>
@@ -12186,7 +12183,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="156" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="156" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B156" s="2" t="s">
         <v>897</v>
       </c>
@@ -12215,7 +12212,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="157" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="157" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B157" s="2" t="s">
         <v>902</v>
       </c>
@@ -12244,7 +12241,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="158" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="158" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B158" s="2" t="s">
         <v>907</v>
       </c>
@@ -12273,7 +12270,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="159" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="159" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B159" s="2" t="s">
         <v>912</v>
       </c>
@@ -12302,7 +12299,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="160" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B160" s="2" t="s">
         <v>917</v>
       </c>
@@ -12331,7 +12328,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="161" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="161" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B161" s="2" t="s">
         <v>922</v>
       </c>
@@ -12360,7 +12357,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="162" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="162" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B162" s="2" t="s">
         <v>927</v>
       </c>
@@ -12389,7 +12386,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="163" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="163" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B163" s="2" t="s">
         <v>932</v>
       </c>
@@ -12418,7 +12415,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="164" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B164" s="2" t="s">
         <v>937</v>
       </c>
@@ -12447,7 +12444,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="165" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B165" s="2" t="s">
         <v>942</v>
       </c>
@@ -12476,7 +12473,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="166" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="166" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B166" s="2" t="s">
         <v>947</v>
       </c>
@@ -12505,7 +12502,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="167" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="167" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B167" s="2" t="s">
         <v>952</v>
       </c>
@@ -12534,7 +12531,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="168" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="168" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B168" s="2" t="s">
         <v>957</v>
       </c>
@@ -12563,7 +12560,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="169" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="169" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B169" s="2" t="s">
         <v>962</v>
       </c>
@@ -12592,7 +12589,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="170" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="170" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B170" s="2" t="s">
         <v>967</v>
       </c>
@@ -12621,7 +12618,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="171" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B171" s="2" t="s">
         <v>972</v>
       </c>
@@ -12650,7 +12647,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="172" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="172" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B172" s="2" t="s">
         <v>977</v>
       </c>
@@ -12679,7 +12676,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="173" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="173" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B173" s="2" t="s">
         <v>982</v>
       </c>
@@ -12708,7 +12705,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="174" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="174" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B174" s="2" t="s">
         <v>987</v>
       </c>
@@ -12737,7 +12734,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="175" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="175" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B175" s="2" t="s">
         <v>992</v>
       </c>
@@ -12766,7 +12763,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="176" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="176" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B176" s="2" t="s">
         <v>997</v>
       </c>
@@ -12795,7 +12792,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="177" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B177" s="2" t="s">
         <v>1002</v>
       </c>
@@ -12824,7 +12821,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="178" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B178" s="2" t="s">
         <v>1007</v>
       </c>
@@ -12853,7 +12850,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="179" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B179" s="2" t="s">
         <v>1012</v>
       </c>
@@ -12882,7 +12879,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="180" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B180" s="2" t="s">
         <v>1017</v>
       </c>
@@ -12911,7 +12908,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="181" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B181" s="2" t="s">
         <v>1022</v>
       </c>
@@ -12940,7 +12937,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="182" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B182" s="2" t="s">
         <v>1027</v>
       </c>
@@ -12969,7 +12966,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="183" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B183" s="2" t="s">
         <v>1032</v>
       </c>
@@ -12998,7 +12995,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="184" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B184" s="2" t="s">
         <v>1037</v>
       </c>
@@ -13027,7 +13024,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="185" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>1042</v>
       </c>
@@ -13059,7 +13056,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="186" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
         <v>1048</v>
       </c>
@@ -13091,7 +13088,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="187" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B187" s="2" t="s">
         <v>1054</v>
       </c>
@@ -13120,7 +13117,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="188" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B188" s="2" t="s">
         <v>1059</v>
       </c>
@@ -13149,7 +13146,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="189" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
         <v>1064</v>
       </c>
@@ -13181,7 +13178,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="190" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B190" s="2" t="s">
         <v>1070</v>
       </c>
@@ -13210,7 +13207,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="191" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B191" s="2" t="s">
         <v>1075</v>
       </c>
@@ -13239,7 +13236,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="192" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B192" s="2" t="s">
         <v>1080</v>
       </c>
@@ -13268,7 +13265,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="193" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B193" s="2" t="s">
         <v>1085</v>
       </c>
@@ -13297,7 +13294,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="194" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B194" s="2" t="s">
         <v>1090</v>
       </c>
@@ -13326,7 +13323,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="195" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B195" s="2" t="s">
         <v>1095</v>
       </c>
@@ -13355,7 +13352,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="196" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B196" s="2" t="s">
         <v>1100</v>
       </c>
@@ -13384,7 +13381,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="197" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B197" s="2" t="s">
         <v>1105</v>
       </c>
@@ -13413,7 +13410,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="198" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B198" s="2" t="s">
         <v>1110</v>
       </c>
@@ -13442,7 +13439,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="199" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B199" s="2" t="s">
         <v>1115</v>
       </c>
@@ -13471,7 +13468,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="200" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B200" s="2" t="s">
         <v>1120</v>
       </c>
@@ -13500,7 +13497,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="201" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B201" s="2" t="s">
         <v>1125</v>
       </c>
@@ -13529,7 +13526,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="202" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B202" s="2" t="s">
         <v>1131</v>
       </c>
@@ -13558,7 +13555,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="203" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B203" s="2" t="s">
         <v>1136</v>
       </c>
@@ -13587,7 +13584,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="204" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B204" s="2" t="s">
         <v>1141</v>
       </c>
@@ -13616,7 +13613,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="205" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
         <v>1146</v>
       </c>
@@ -13648,7 +13645,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="206" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B206" s="2" t="s">
         <v>1152</v>
       </c>
@@ -13677,7 +13674,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="207" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B207" s="2" t="s">
         <v>1157</v>
       </c>
@@ -13706,7 +13703,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="208" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B208" s="2" t="s">
         <v>1162</v>
       </c>
@@ -13735,7 +13732,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="209" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B209" s="2" t="s">
         <v>1167</v>
       </c>
@@ -13764,7 +13761,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="210" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
         <v>1172</v>
       </c>
@@ -13799,7 +13796,7 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="211" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B211" s="2" t="s">
         <v>1178</v>
       </c>
@@ -13828,7 +13825,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="212" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B212" s="2" t="s">
         <v>1183</v>
       </c>
@@ -13857,7 +13854,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="213" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B213" s="2" t="s">
         <v>1188</v>
       </c>
@@ -13886,7 +13883,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="214" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B214" s="2" t="s">
         <v>1193</v>
       </c>
@@ -13915,7 +13912,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="215" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B215" s="2" t="s">
         <v>1198</v>
       </c>
@@ -13944,7 +13941,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="216" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B216" s="2" t="s">
         <v>1203</v>
       </c>
@@ -13973,7 +13970,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="217" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B217" s="2" t="s">
         <v>1208</v>
       </c>
@@ -14002,7 +13999,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="218" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B218" s="2" t="s">
         <v>1213</v>
       </c>
@@ -14031,7 +14028,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="219" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B219" s="2" t="s">
         <v>1218</v>
       </c>
@@ -14060,7 +14057,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="220" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B220" s="2" t="s">
         <v>1223</v>
       </c>
@@ -14089,7 +14086,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="221" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
         <v>1228</v>
       </c>
@@ -14121,7 +14118,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="222" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B222" s="2" t="s">
         <v>1234</v>
       </c>
@@ -14153,7 +14150,7 @@
         <v>1415</v>
       </c>
     </row>
-    <row r="223" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B223" s="2" t="s">
         <v>1239</v>
       </c>
@@ -14182,7 +14179,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="224" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B224" s="2" t="s">
         <v>1244</v>
       </c>
@@ -14211,7 +14208,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="225" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B225" s="2" t="s">
         <v>1249</v>
       </c>
@@ -14240,7 +14237,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="226" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B226" s="2" t="s">
         <v>1254</v>
       </c>
@@ -14269,7 +14266,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="227" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B227" s="2" t="s">
         <v>1259</v>
       </c>
@@ -14298,7 +14295,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="228" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B228" s="2" t="s">
         <v>1264</v>
       </c>
@@ -14327,7 +14324,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="229" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B229" s="2" t="s">
         <v>1269</v>
       </c>
@@ -14356,7 +14353,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="230" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
         <v>1274</v>
       </c>
@@ -14388,7 +14385,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="231" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B231" s="2" t="s">
         <v>1280</v>
       </c>
@@ -14417,7 +14414,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="232" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B232" s="2" t="s">
         <v>1285</v>
       </c>
@@ -14446,7 +14443,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="233" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B233" s="2" t="s">
         <v>1290</v>
       </c>
@@ -14475,7 +14472,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="234" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B234" s="2" t="s">
         <v>1295</v>
       </c>
@@ -14504,7 +14501,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="235" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B235" s="2" t="s">
         <v>1300</v>
       </c>
@@ -14533,7 +14530,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="236" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B236" s="2" t="s">
         <v>1305</v>
       </c>
@@ -14562,7 +14559,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="237" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B237" s="2" t="s">
         <v>1310</v>
       </c>
@@ -14591,7 +14588,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="238" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B238" s="2" t="s">
         <v>1315</v>
       </c>
@@ -14620,7 +14617,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="239" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B239" s="2" t="s">
         <v>1320</v>
       </c>
@@ -14649,7 +14646,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="240" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B240" s="2" t="s">
         <v>1325</v>
       </c>
@@ -14681,7 +14678,7 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="241" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B241" s="2" t="s">
         <v>1330</v>
       </c>
@@ -14710,7 +14707,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="242" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B242" s="2" t="s">
         <v>1335</v>
       </c>
@@ -14742,7 +14739,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="243" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A243" s="2" t="s">
         <v>1340</v>
       </c>
@@ -14774,7 +14771,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="244" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A244" s="2" t="s">
         <v>1346</v>
       </c>
@@ -14806,7 +14803,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="245" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A245" s="2" t="s">
         <v>1352</v>
       </c>
@@ -14838,7 +14835,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="246" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B246" s="2" t="s">
         <v>1358</v>
       </c>
@@ -14870,7 +14867,7 @@
         <v>1413</v>
       </c>
     </row>
-    <row r="247" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B247" s="2" t="s">
         <v>1363</v>
       </c>
@@ -14902,7 +14899,7 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="248" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A248" s="2" t="s">
         <v>1368</v>
       </c>
@@ -14934,7 +14931,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="249" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A249" s="2" t="s">
         <v>1374</v>
       </c>
@@ -14969,7 +14966,7 @@
         <v>1410</v>
       </c>
     </row>
-    <row r="250" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A250" s="2" t="s">
         <v>1381</v>
       </c>
@@ -15004,7 +15001,7 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="251" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A251" s="2" t="s">
         <v>1387</v>
       </c>
@@ -15036,7 +15033,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="252" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A252" s="2" t="s">
         <v>1393</v>
       </c>
@@ -15068,7 +15065,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="253" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A253" s="2" t="s">
         <v>1399</v>
       </c>
@@ -15103,7 +15100,7 @@
         <v>1407</v>
       </c>
     </row>
-    <row r="254" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A254" s="2" t="s">
         <v>1430</v>
       </c>
@@ -15132,10 +15129,10 @@
         <v>1435</v>
       </c>
       <c r="J254" s="3" t="s">
-        <v>2272</v>
-      </c>
-    </row>
-    <row r="255" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+        <v>1405</v>
+      </c>
+    </row>
+    <row r="255" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A255" s="2" t="s">
         <v>1436</v>
       </c>
@@ -15167,7 +15164,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="256" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:11" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A256" s="2" t="s">
         <v>1442</v>
       </c>
@@ -15199,7 +15196,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="257" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A257" s="2" t="s">
         <v>1448</v>
       </c>
@@ -15231,7 +15228,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="258" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A258" s="2" t="s">
         <v>1454</v>
       </c>
@@ -15263,7 +15260,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="259" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A259" s="2" t="s">
         <v>1460</v>
       </c>
@@ -15295,7 +15292,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="260" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B260" s="2" t="s">
         <v>1466</v>
       </c>
@@ -15324,7 +15321,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="261" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A261" s="2" t="s">
         <v>1471</v>
       </c>
@@ -15356,7 +15353,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="262" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A262" s="2" t="s">
         <v>1477</v>
       </c>
@@ -15388,7 +15385,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="263" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A263" s="2" t="s">
         <v>1483</v>
       </c>
@@ -15420,7 +15417,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="264" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A264" s="2" t="s">
         <v>1489</v>
       </c>
@@ -15452,7 +15449,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="265" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A265" s="2" t="s">
         <v>1495</v>
       </c>
@@ -15484,7 +15481,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="266" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A266" s="2" t="s">
         <v>1501</v>
       </c>
@@ -15516,7 +15513,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="267" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A267" s="2" t="s">
         <v>1507</v>
       </c>
@@ -15548,7 +15545,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="268" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A268" s="2" t="s">
         <v>1513</v>
       </c>
@@ -15580,7 +15577,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="269" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A269" s="2" t="s">
         <v>1519</v>
       </c>
@@ -15612,7 +15609,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="270" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A270" s="2" t="s">
         <v>1525</v>
       </c>
@@ -15644,7 +15641,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="271" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A271" s="2" t="s">
         <v>1531</v>
       </c>
@@ -15676,7 +15673,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="272" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A272" s="2" t="s">
         <v>1537</v>
       </c>
@@ -15708,7 +15705,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="273" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A273" s="2" t="s">
         <v>1543</v>
       </c>
@@ -15740,7 +15737,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="274" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A274" s="2" t="s">
         <v>1549</v>
       </c>
@@ -15772,7 +15769,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="275" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A275" s="2" t="s">
         <v>1555</v>
       </c>
@@ -15804,7 +15801,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="276" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A276" s="2" t="s">
         <v>1561</v>
       </c>
@@ -15836,7 +15833,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="277" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B277" s="2" t="s">
         <v>1567</v>
       </c>
@@ -15865,7 +15862,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="278" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A278" s="2" t="s">
         <v>1572</v>
       </c>
@@ -15897,7 +15894,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="279" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A279" s="2" t="s">
         <v>1578</v>
       </c>
@@ -15929,7 +15926,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="280" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A280" s="2" t="s">
         <v>1584</v>
       </c>
@@ -15961,7 +15958,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="281" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A281" s="2" t="s">
         <v>1590</v>
       </c>
@@ -15993,7 +15990,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="282" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B282" s="2" t="s">
         <v>1596</v>
       </c>
@@ -16022,7 +16019,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="283" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A283" s="2" t="s">
         <v>1601</v>
       </c>
@@ -16054,7 +16051,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="284" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A284" s="2" t="s">
         <v>1607</v>
       </c>
@@ -16086,7 +16083,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="285" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A285" s="2" t="s">
         <v>1613</v>
       </c>
@@ -16118,7 +16115,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="286" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A286" s="2" t="s">
         <v>1619</v>
       </c>
@@ -16150,7 +16147,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="287" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A287" s="2" t="s">
         <v>1625</v>
       </c>
@@ -16182,7 +16179,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="288" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A288" s="2" t="s">
         <v>1631</v>
       </c>
@@ -16214,7 +16211,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="289" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A289" s="2" t="s">
         <v>1637</v>
       </c>
@@ -16246,7 +16243,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="290" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A290" s="2" t="s">
         <v>1643</v>
       </c>
@@ -16278,7 +16275,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="291" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A291" s="2" t="s">
         <v>1649</v>
       </c>
@@ -16310,7 +16307,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="292" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B292" s="2" t="s">
         <v>1655</v>
       </c>
@@ -16339,7 +16336,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="293" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A293" s="2" t="s">
         <v>1660</v>
       </c>
@@ -16371,7 +16368,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="294" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A294" s="2" t="s">
         <v>1666</v>
       </c>
@@ -16403,7 +16400,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="295" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B295" s="2" t="s">
         <v>1672</v>
       </c>
@@ -16432,7 +16429,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="296" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A296" s="2" t="s">
         <v>1677</v>
       </c>
@@ -16464,7 +16461,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="297" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A297" s="2" t="s">
         <v>1683</v>
       </c>
@@ -16496,7 +16493,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="298" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A298" s="2" t="s">
         <v>1689</v>
       </c>
@@ -16528,7 +16525,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="299" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A299" s="2" t="s">
         <v>1695</v>
       </c>
@@ -16560,7 +16557,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="300" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A300" s="2" t="s">
         <v>1701</v>
       </c>
@@ -16592,7 +16589,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="301" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A301" s="2" t="s">
         <v>1707</v>
       </c>
@@ -16624,7 +16621,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="302" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A302" s="2" t="s">
         <v>1713</v>
       </c>
@@ -16656,7 +16653,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="303" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A303" s="2" t="s">
         <v>1719</v>
       </c>
@@ -16688,7 +16685,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="304" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A304" s="2" t="s">
         <v>1725</v>
       </c>
@@ -16720,7 +16717,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="305" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A305" s="2" t="s">
         <v>1731</v>
       </c>
@@ -16752,7 +16749,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="306" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A306" s="2" t="s">
         <v>1737</v>
       </c>
@@ -16784,7 +16781,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="307" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A307" s="2" t="s">
         <v>1743</v>
       </c>
@@ -16816,7 +16813,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="308" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B308" s="2" t="s">
         <v>1749</v>
       </c>
@@ -16845,7 +16842,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="309" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B309" s="2" t="s">
         <v>1754</v>
       </c>
@@ -16874,7 +16871,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="310" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B310" s="2" t="s">
         <v>1759</v>
       </c>
@@ -16903,7 +16900,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="311" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B311" s="2" t="s">
         <v>1764</v>
       </c>
@@ -16932,7 +16929,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="312" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B312" s="2" t="s">
         <v>1769</v>
       </c>
@@ -16961,7 +16958,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="313" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B313" s="2" t="s">
         <v>1774</v>
       </c>
@@ -16990,7 +16987,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="314" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B314" s="2" t="s">
         <v>1779</v>
       </c>
@@ -17019,7 +17016,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="315" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B315" s="2" t="s">
         <v>1784</v>
       </c>
@@ -17048,7 +17045,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="316" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B316" s="2" t="s">
         <v>1789</v>
       </c>
@@ -17077,7 +17074,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="317" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B317" s="2" t="s">
         <v>1794</v>
       </c>
@@ -17106,7 +17103,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="318" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B318" s="2" t="s">
         <v>1799</v>
       </c>
@@ -17135,7 +17132,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="319" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B319" s="2" t="s">
         <v>1804</v>
       </c>
@@ -17164,7 +17161,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="320" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B320" s="2" t="s">
         <v>1809</v>
       </c>
@@ -17193,7 +17190,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="321" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="321" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B321" s="2" t="s">
         <v>1814</v>
       </c>
@@ -17222,7 +17219,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="322" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="322" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B322" s="2" t="s">
         <v>1819</v>
       </c>
@@ -17251,7 +17248,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="323" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="323" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B323" s="2" t="s">
         <v>1824</v>
       </c>
@@ -17280,7 +17277,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="324" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="324" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B324" s="2" t="s">
         <v>1829</v>
       </c>
@@ -17309,7 +17306,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="325" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="325" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B325" s="2" t="s">
         <v>1834</v>
       </c>
@@ -17338,7 +17335,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="326" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="326" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B326" s="2" t="s">
         <v>1839</v>
       </c>
@@ -17367,7 +17364,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="327" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="327" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B327" s="2" t="s">
         <v>1844</v>
       </c>
@@ -17396,7 +17393,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="328" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="328" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B328" s="2" t="s">
         <v>1849</v>
       </c>
@@ -17425,7 +17422,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="329" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="329" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B329" s="2" t="s">
         <v>1854</v>
       </c>
@@ -17454,7 +17451,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="330" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="330" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B330" s="2" t="s">
         <v>1859</v>
       </c>
@@ -17483,7 +17480,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="331" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="331" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B331" s="2" t="s">
         <v>1864</v>
       </c>
@@ -17512,7 +17509,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="332" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="332" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B332" s="2" t="s">
         <v>1869</v>
       </c>
@@ -17541,7 +17538,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="333" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="333" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B333" s="2" t="s">
         <v>1874</v>
       </c>
@@ -17570,7 +17567,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="334" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="334" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B334" s="2" t="s">
         <v>1879</v>
       </c>
@@ -17599,7 +17596,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="335" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="335" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B335" s="2" t="s">
         <v>1884</v>
       </c>
@@ -17628,7 +17625,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="336" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="336" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B336" s="2" t="s">
         <v>1889</v>
       </c>
@@ -17657,7 +17654,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="337" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B337" s="2" t="s">
         <v>1894</v>
       </c>
@@ -17686,7 +17683,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="338" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B338" s="2" t="s">
         <v>1899</v>
       </c>
@@ -17715,7 +17712,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="339" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B339" s="2" t="s">
         <v>1904</v>
       </c>
@@ -17744,7 +17741,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="340" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B340" s="2" t="s">
         <v>1909</v>
       </c>
@@ -17773,7 +17770,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="341" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B341" s="2" t="s">
         <v>1914</v>
       </c>
@@ -17802,7 +17799,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="342" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B342" s="2" t="s">
         <v>1919</v>
       </c>
@@ -17831,7 +17828,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="343" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B343" s="2" t="s">
         <v>1924</v>
       </c>
@@ -17860,7 +17857,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="344" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A344" s="2" t="s">
         <v>1929</v>
       </c>
@@ -17892,7 +17889,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="345" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B345" s="2" t="s">
         <v>1935</v>
       </c>
@@ -17921,7 +17918,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="346" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B346" s="2" t="s">
         <v>1940</v>
       </c>
@@ -17950,7 +17947,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="347" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B347" s="2" t="s">
         <v>1945</v>
       </c>
@@ -17979,7 +17976,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="348" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B348" s="2" t="s">
         <v>1950</v>
       </c>
@@ -18008,7 +18005,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="349" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B349" s="2" t="s">
         <v>1955</v>
       </c>
@@ -18037,7 +18034,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="350" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B350" s="2" t="s">
         <v>1960</v>
       </c>
@@ -18066,7 +18063,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="351" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B351" s="2" t="s">
         <v>1965</v>
       </c>
@@ -18095,7 +18092,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="352" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B352" s="2" t="s">
         <v>1970</v>
       </c>
@@ -18124,7 +18121,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="353" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="353" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B353" s="2" t="s">
         <v>1975</v>
       </c>
@@ -18153,7 +18150,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="354" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="354" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B354" s="2" t="s">
         <v>1980</v>
       </c>
@@ -18182,7 +18179,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="355" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="355" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B355" s="2" t="s">
         <v>1985</v>
       </c>
@@ -18211,7 +18208,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="356" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="356" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B356" s="2" t="s">
         <v>1990</v>
       </c>
@@ -18240,7 +18237,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="357" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="357" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B357" s="2" t="s">
         <v>1995</v>
       </c>
@@ -18269,7 +18266,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="358" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="358" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B358" s="2" t="s">
         <v>2000</v>
       </c>
@@ -18298,7 +18295,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="359" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="359" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B359" s="2" t="s">
         <v>2005</v>
       </c>
@@ -18327,7 +18324,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="360" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="360" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B360" s="2" t="s">
         <v>2010</v>
       </c>
@@ -18356,7 +18353,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="361" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="361" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B361" s="2" t="s">
         <v>2015</v>
       </c>
@@ -18385,7 +18382,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="362" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="362" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B362" s="2" t="s">
         <v>2020</v>
       </c>
@@ -18414,7 +18411,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="363" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="363" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B363" s="2" t="s">
         <v>2025</v>
       </c>
@@ -18443,7 +18440,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="364" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="364" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B364" s="2" t="s">
         <v>2030</v>
       </c>
@@ -18472,7 +18469,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="365" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="365" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B365" s="2" t="s">
         <v>2035</v>
       </c>
@@ -18501,7 +18498,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="366" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="366" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B366" s="2" t="s">
         <v>2040</v>
       </c>
@@ -18530,7 +18527,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="367" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="367" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B367" s="2" t="s">
         <v>2045</v>
       </c>
@@ -18559,7 +18556,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="368" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="368" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B368" s="2" t="s">
         <v>2050</v>
       </c>
@@ -18588,7 +18585,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="369" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="369" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B369" s="2" t="s">
         <v>2055</v>
       </c>
@@ -18617,7 +18614,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="370" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="370" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B370" s="2" t="s">
         <v>2060</v>
       </c>
@@ -18646,7 +18643,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="371" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="371" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B371" s="2" t="s">
         <v>2065</v>
       </c>
@@ -18675,7 +18672,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="372" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="372" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B372" s="2" t="s">
         <v>2070</v>
       </c>
@@ -18704,7 +18701,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="373" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="373" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B373" s="2" t="s">
         <v>2075</v>
       </c>
@@ -18733,7 +18730,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="374" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="374" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B374" s="2" t="s">
         <v>2080</v>
       </c>
@@ -18762,7 +18759,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="375" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="375" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B375" s="2" t="s">
         <v>2085</v>
       </c>
@@ -18791,7 +18788,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="376" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="376" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B376" s="2" t="s">
         <v>2090</v>
       </c>
@@ -18820,7 +18817,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="377" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="377" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B377" s="2" t="s">
         <v>2095</v>
       </c>
@@ -18849,7 +18846,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="378" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="378" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B378" s="2" t="s">
         <v>2100</v>
       </c>
@@ -18878,7 +18875,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="379" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="379" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B379" s="2" t="s">
         <v>2105</v>
       </c>
@@ -18907,7 +18904,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="380" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="380" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B380" s="2" t="s">
         <v>2110</v>
       </c>
@@ -18936,7 +18933,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="381" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="381" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B381" s="2" t="s">
         <v>2115</v>
       </c>
@@ -18965,7 +18962,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="382" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="382" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B382" s="2" t="s">
         <v>2120</v>
       </c>
@@ -18994,7 +18991,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="383" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="383" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B383" s="2" t="s">
         <v>2125</v>
       </c>
@@ -19023,7 +19020,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="384" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="384" spans="2:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B384" s="2" t="s">
         <v>2130</v>
       </c>
@@ -19052,7 +19049,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="385" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B385" s="2" t="s">
         <v>2135</v>
       </c>
@@ -19081,7 +19078,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="386" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A386" s="2" t="s">
         <v>2140</v>
       </c>
@@ -19113,7 +19110,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="387" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A387" s="2" t="s">
         <v>2146</v>
       </c>
@@ -19145,7 +19142,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="388" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B388" s="2" t="s">
         <v>2152</v>
       </c>
@@ -19174,7 +19171,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="389" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B389" s="2" t="s">
         <v>2157</v>
       </c>
@@ -19203,7 +19200,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="390" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B390" s="2" t="s">
         <v>2162</v>
       </c>
@@ -19232,7 +19229,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="391" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B391" s="2" t="s">
         <v>2167</v>
       </c>
@@ -19261,7 +19258,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="392" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B392" s="2" t="s">
         <v>2172</v>
       </c>
@@ -19290,7 +19287,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="393" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B393" s="2" t="s">
         <v>2177</v>
       </c>
@@ -19319,7 +19316,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="394" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B394" s="2" t="s">
         <v>2182</v>
       </c>
@@ -19348,7 +19345,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="395" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A395" s="2" t="s">
         <v>2187</v>
       </c>
@@ -19380,7 +19377,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="396" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A396" s="2" t="s">
         <v>2193</v>
       </c>
@@ -19412,7 +19409,7 @@
         <v>1408</v>
       </c>
     </row>
-    <row r="397" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A397" s="2" t="s">
         <v>2199</v>
       </c>
@@ -19444,7 +19441,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="398" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B398" s="2" t="s">
         <v>2205</v>
       </c>
@@ -19473,7 +19470,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="399" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B399" s="2" t="s">
         <v>2211</v>
       </c>
@@ -19502,7 +19499,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="400" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A400" s="2" t="s">
         <v>2216</v>
       </c>
@@ -19534,7 +19531,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="401" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A401" s="2" t="s">
         <v>2222</v>
       </c>
@@ -19566,7 +19563,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="402" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A402" s="2" t="s">
         <v>2230</v>
       </c>
@@ -19598,7 +19595,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="403" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A403" s="2" t="s">
         <v>2236</v>
       </c>
@@ -19630,7 +19627,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="404" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A404" s="2" t="s">
         <v>2242</v>
       </c>
@@ -19662,7 +19659,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="405" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A405" s="2" t="s">
         <v>2248</v>
       </c>
@@ -19694,7 +19691,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="406" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A406" s="2" t="s">
         <v>2254</v>
       </c>
@@ -19726,7 +19723,7 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="407" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A407" s="2" t="s">
         <v>2260</v>
       </c>
@@ -19758,7 +19755,7 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="408" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:10" ht="180" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A408" s="2" t="s">
         <v>2266</v>
       </c>

</xml_diff>